<commit_message>
Dummy change in Bill
</commit_message>
<xml_diff>
--- a/Bill of Materials/Bill Of Materials.xlsx
+++ b/Bill of Materials/Bill Of Materials.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -264,7 +264,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -299,7 +299,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -512,7 +512,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +636,9 @@
         <v>20</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2">
+        <v>9803002</v>
+      </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2">

</xml_diff>